<commit_message>
updated dates in excel file
</commit_message>
<xml_diff>
--- a/Step-3-4/result_FIRSTNAME_LASTNAME.xlsx
+++ b/Step-3-4/result_FIRSTNAME_LASTNAME.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moene001\OneDrive - Wageningen University &amp; Research\Documents\onderwijs\vakken\Hupsel\2021\04_uitwerking\Step-3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moene001\OneDrive - Wageningen University &amp; Research\Documents\onderwijs\vakken\Hupsel\git\hupsel\Step-3-4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A30A8519-FE1C-42CF-8C50-4836CDE02465}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5B0A58-0CF9-49D9-9162-7D2579017CBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{13B91B18-642C-4F09-AB8F-2F8310B40AB1}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{13B91B18-642C-4F09-AB8F-2F8310B40AB1}"/>
   </bookViews>
   <sheets>
     <sheet name="ET actual of Hupsel catchment" sheetId="1" r:id="rId1"/>
@@ -431,12 +431,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF39021B-3A5B-422F-80D4-00C52C6C5E00}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="16.90625" customWidth="1"/>
-    <col min="2" max="2" width="24.453125" customWidth="1"/>
+    <col min="1" max="1" width="16.88671875" customWidth="1"/>
+    <col min="2" max="2" width="24.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -457,157 +459,182 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>44317</v>
+        <v>44675</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
-        <v>44318</v>
+        <f>A3+1</f>
+        <v>44676</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
-        <v>44319</v>
+        <f t="shared" ref="A5:A28" si="0">A4+1</f>
+        <v>44677</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
-        <v>44320</v>
+        <f t="shared" si="0"/>
+        <v>44678</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
-        <v>44321</v>
+        <f t="shared" si="0"/>
+        <v>44679</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
-        <v>44322</v>
+        <f t="shared" si="0"/>
+        <v>44680</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
-        <v>44323</v>
+        <f t="shared" si="0"/>
+        <v>44681</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
-        <v>44324</v>
+        <f t="shared" si="0"/>
+        <v>44682</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
-        <v>44325</v>
+        <f t="shared" si="0"/>
+        <v>44683</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
-        <v>44326</v>
+        <f t="shared" si="0"/>
+        <v>44684</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
-        <v>44327</v>
+        <f t="shared" si="0"/>
+        <v>44685</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
-        <v>44328</v>
+        <f t="shared" si="0"/>
+        <v>44686</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
-        <v>44329</v>
+        <f t="shared" si="0"/>
+        <v>44687</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
-        <v>44330</v>
+        <f t="shared" si="0"/>
+        <v>44688</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
-        <v>44331</v>
+        <f t="shared" si="0"/>
+        <v>44689</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
-        <v>44332</v>
+        <f t="shared" si="0"/>
+        <v>44690</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
-        <v>44333</v>
+        <f t="shared" si="0"/>
+        <v>44691</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1">
-        <v>44334</v>
+        <f t="shared" si="0"/>
+        <v>44692</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1">
-        <v>44335</v>
+        <f t="shared" si="0"/>
+        <v>44693</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1">
-        <v>44336</v>
+        <f t="shared" si="0"/>
+        <v>44694</v>
       </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1">
-        <v>44337</v>
+        <f t="shared" si="0"/>
+        <v>44695</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1">
-        <v>44338</v>
+        <f t="shared" si="0"/>
+        <v>44696</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" s="1">
-        <v>44339</v>
+        <f t="shared" si="0"/>
+        <v>44697</v>
       </c>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1">
-        <v>44340</v>
+        <f t="shared" si="0"/>
+        <v>44698</v>
       </c>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="1">
-        <v>44341</v>
+        <f t="shared" si="0"/>
+        <v>44699</v>
       </c>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="1">
-        <v>44342</v>
+        <f t="shared" si="0"/>
+        <v>44700</v>
       </c>
       <c r="B28" s="2"/>
     </row>

</xml_diff>

<commit_message>
* updated step 1 and 2 based on the first ron of the practical * prepared new KNMI data for 2023 * updated catchment ET answer sheet
</commit_message>
<xml_diff>
--- a/Step-3-4/result_FIRSTNAME_LASTNAME.xlsx
+++ b/Step-3-4/result_FIRSTNAME_LASTNAME.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\moene001\OneDrive - Wageningen University &amp; Research\Documents\onderwijs\vakken\Hupsel\git\hupsel\Step-3-4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://wageningenur4-my.sharepoint.com/personal/arnold_moene_wur_nl/Documents/Documents/onderwijs/vakken/Hupsel/2023/04_uitwerking/Fluxes-2/Step-3+4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5B0A58-0CF9-49D9-9162-7D2579017CBF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A30A8519-FE1C-42CF-8C50-4836CDE02465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C1BF83FF-E403-4C3B-99F6-2D81A2627FB8}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{13B91B18-642C-4F09-AB8F-2F8310B40AB1}"/>
+    <workbookView xWindow="30240" yWindow="1440" windowWidth="21600" windowHeight="11430" xr2:uid="{13B91B18-642C-4F09-AB8F-2F8310B40AB1}"/>
   </bookViews>
   <sheets>
     <sheet name="ET actual of Hupsel catchment" sheetId="1" r:id="rId1"/>
@@ -431,9 +431,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF39021B-3A5B-422F-80D4-00C52C6C5E00}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -459,183 +457,171 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1">
-        <v>44675</v>
+        <v>45053</v>
       </c>
       <c r="B3" s="2"/>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1">
         <f>A3+1</f>
-        <v>44676</v>
+        <v>45054</v>
       </c>
       <c r="B4" s="2"/>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="1">
         <f t="shared" ref="A5:A28" si="0">A4+1</f>
-        <v>44677</v>
+        <v>45055</v>
       </c>
       <c r="B5" s="2"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1">
         <f t="shared" si="0"/>
-        <v>44678</v>
+        <v>45056</v>
       </c>
       <c r="B6" s="2"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1">
         <f t="shared" si="0"/>
-        <v>44679</v>
+        <v>45057</v>
       </c>
       <c r="B7" s="2"/>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="1">
         <f t="shared" si="0"/>
-        <v>44680</v>
+        <v>45058</v>
       </c>
       <c r="B8" s="2"/>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="1">
         <f t="shared" si="0"/>
-        <v>44681</v>
+        <v>45059</v>
       </c>
       <c r="B9" s="2"/>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="1">
         <f t="shared" si="0"/>
-        <v>44682</v>
+        <v>45060</v>
       </c>
       <c r="B10" s="2"/>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="1">
         <f t="shared" si="0"/>
-        <v>44683</v>
+        <v>45061</v>
       </c>
       <c r="B11" s="2"/>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1">
         <f t="shared" si="0"/>
-        <v>44684</v>
+        <v>45062</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1">
         <f t="shared" si="0"/>
-        <v>44685</v>
+        <v>45063</v>
       </c>
       <c r="B13" s="2"/>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" s="1">
         <f t="shared" si="0"/>
-        <v>44686</v>
+        <v>45064</v>
       </c>
       <c r="B14" s="2"/>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="1">
         <f t="shared" si="0"/>
-        <v>44687</v>
+        <v>45065</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
-        <v>44688</v>
+        <v>45066</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
-        <v>44689</v>
+        <v>45067</v>
       </c>
       <c r="B17" s="2"/>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
-        <v>44690</v>
+        <v>45068</v>
       </c>
       <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
-        <v>44691</v>
+        <v>45069</v>
       </c>
       <c r="B19" s="2"/>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
-        <v>44692</v>
+        <v>45070</v>
       </c>
       <c r="B20" s="2"/>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
-        <v>44693</v>
+        <v>45071</v>
       </c>
       <c r="B21" s="2"/>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
-        <v>44694</v>
+        <v>45072</v>
       </c>
       <c r="B22" s="2"/>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
-        <v>44695</v>
+        <v>45073</v>
       </c>
       <c r="B23" s="2"/>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
-        <v>44696</v>
+        <v>45074</v>
       </c>
       <c r="B24" s="2"/>
     </row>
     <row r="25" spans="1:2">
-      <c r="A25" s="1">
-        <f t="shared" si="0"/>
-        <v>44697</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="2"/>
     </row>
     <row r="26" spans="1:2">
-      <c r="A26" s="1">
-        <f t="shared" si="0"/>
-        <v>44698</v>
-      </c>
+      <c r="A26" s="1"/>
       <c r="B26" s="2"/>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="1">
-        <f t="shared" si="0"/>
-        <v>44699</v>
-      </c>
+      <c r="A27" s="1"/>
       <c r="B27" s="2"/>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="1">
-        <f t="shared" si="0"/>
-        <v>44700</v>
-      </c>
+      <c r="A28" s="1"/>
       <c r="B28" s="2"/>
     </row>
   </sheetData>

</xml_diff>